<commit_message>
analyzing and all with new data
</commit_message>
<xml_diff>
--- a/ghz-predictors.xlsx
+++ b/ghz-predictors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerry\repos\2022-638\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C76196B-3E16-4197-A9E5-FC3966B318E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E595206C-D6CF-48C6-8AA2-DD851CCF5602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="16201" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="313">
   <si>
     <t>name</t>
   </si>
@@ -954,6 +954,12 @@
   </si>
   <si>
     <t>code</t>
+  </si>
+  <si>
+    <t>Quarterly return on equity</t>
+  </si>
+  <si>
+    <t>Earnings before extraordinary items divided by lagged shareholders' equity</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C71" workbookViewId="0">
       <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
@@ -2481,6 +2487,12 @@
       <c r="A83" t="s">
         <v>249</v>
       </c>
+      <c r="B83" t="s">
+        <v>311</v>
+      </c>
+      <c r="C83" t="s">
+        <v>312</v>
+      </c>
       <c r="L83" t="s">
         <v>81</v>
       </c>

</xml_diff>